<commit_message>
action plan co list task . sap xep theo uu tien mau do truoc. c xem thiet ke 1 trang thong bao loi nhe. tham khao trang loi vnexpress.
</commit_message>
<xml_diff>
--- a/resources/documents/ActionPlan.xlsx
+++ b/resources/documents/ActionPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="62">
   <si>
     <t>STT</t>
   </si>
@@ -85,6 +85,123 @@
   </si>
   <si>
     <t>Thiết lập môi trường ứng dụng + Tìm hiểu SEO</t>
+  </si>
+  <si>
+    <t>Công việc tồn đọng</t>
+  </si>
+  <si>
+    <t>Loại</t>
+  </si>
+  <si>
+    <t>Ưu tiên</t>
+  </si>
+  <si>
+    <t>Phần</t>
+  </si>
+  <si>
+    <t>Phân quyền user admin (BTV, sysadmin, admin)</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Quản lý mục Kết bạn (account, bình luận)</t>
+  </si>
+  <si>
+    <t>Quản lý porlet quảng cáo (xml, bên column right, banner)</t>
+  </si>
+  <si>
+    <t>Tìm kiếm quảng cáo</t>
+  </si>
+  <si>
+    <t>site func</t>
+  </si>
+  <si>
+    <t>Tìm kiếm profile</t>
+  </si>
+  <si>
+    <t>đăng ký profile</t>
+  </si>
+  <si>
+    <t>Quản ly danh mục MTV (video)</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>Post video (upload --&gt; sau đó add link vào DB)</t>
+  </si>
+  <si>
+    <t>Page MTV (phân loại theo category)</t>
+  </si>
+  <si>
+    <t>Lỗi nivo slide tại porlet hot new</t>
+  </si>
+  <si>
+    <t>bug</t>
+  </si>
+  <si>
+    <t>Lỗi khi post bài (thỉnh thoảng) An error occurred while updating the entries. See the InnerException for details</t>
+  </si>
+  <si>
+    <t>lỗi giao diện (căn plet tin nổi bật sao cho = tin mới nhât)</t>
+  </si>
+  <si>
+    <t>Lỗi search có ký tự đặc biệt</t>
+  </si>
+  <si>
+    <t>Trang thông báo lỗi</t>
+  </si>
+  <si>
+    <t>Lỗi phần dự báo thời tiết ( chưa phiên dịch 1 số từ)</t>
+  </si>
+  <si>
+    <t>Lỗi nhập liệu potentially dangerous Request</t>
+  </si>
+  <si>
+    <t>all input form</t>
+  </si>
+  <si>
+    <t>Logo theo ý tưởng (tờ báo + chuột quang =&gt; báo đtử)</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>Quản lý logo, banner (cho phép thay đổi)</t>
+  </si>
+  <si>
+    <t>Hiện trạng</t>
+  </si>
+  <si>
+    <t>Phụ trách</t>
+  </si>
+  <si>
+    <t>chưa làm</t>
+  </si>
+  <si>
+    <t>duynp</t>
+  </si>
+  <si>
+    <t>cuongnq</t>
+  </si>
+  <si>
+    <t>RSS</t>
+  </si>
+  <si>
+    <t>Mo ta</t>
+  </si>
+  <si>
+    <t>C design 1 trang thong bao loi nhe</t>
+  </si>
+  <si>
+    <t>c research xem giai phap linq</t>
+  </si>
+  <si>
+    <t>thiet ke form</t>
   </si>
 </sst>
 </file>
@@ -94,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +232,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,8 +271,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -165,11 +313,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -196,6 +370,34 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,25 +692,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H14"/>
+  <dimension ref="A2:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" activeCellId="3" sqref="H4 H6 H9 H12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23:K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="46.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="54.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="17.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="20.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -534,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -553,11 +758,11 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="3">
-        <f>D3-C3+1</f>
+        <f t="shared" ref="H3:H14" si="0">D3-C3+1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -576,11 +781,11 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="3">
-        <f>D4-C4+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:11">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -599,11 +804,11 @@
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="3">
-        <f>D5-C5+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:11">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -624,11 +829,11 @@
         <v>40617</v>
       </c>
       <c r="H6" s="11">
-        <f>D6-C6+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:11">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -647,11 +852,11 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="3">
-        <f>D7-C7+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:11">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -670,11 +875,11 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3">
-        <f>D8-C8+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:11">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -695,11 +900,11 @@
         <v>40624</v>
       </c>
       <c r="H9" s="11">
-        <f>D9-C9+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:11">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -718,11 +923,11 @@
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3">
-        <f>D10-C10+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:11">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -741,11 +946,11 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="3">
-        <f>D11-C11+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:11">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -766,11 +971,11 @@
         <v>40629</v>
       </c>
       <c r="H12" s="11">
-        <f>D12-C12+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:11">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -789,11 +994,11 @@
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="3">
-        <f>D13-C13+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:11">
       <c r="A14" s="13">
         <v>12</v>
       </c>
@@ -812,11 +1017,603 @@
         <v>40633</v>
       </c>
       <c r="H14" s="14">
-        <f>D14-C14+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="27"/>
+      <c r="J16" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="23">
+        <v>1</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="24">
+        <v>4</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="23">
+        <v>2</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="24">
+        <v>4</v>
+      </c>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="10">
+        <v>3</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="11">
+        <v>2</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="20">
+        <v>4</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="21">
+        <v>3</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="21"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="13">
+        <v>5</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="14">
+        <v>1</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" s="29"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="13">
+        <v>6</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="14">
+        <v>1</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="14"/>
+      <c r="J22" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="K22" s="29"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="13">
+        <v>7</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="14">
+        <v>1</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="K23" s="29"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="20">
+        <v>8</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="21">
+        <v>3</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="21"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="27"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="20">
+        <v>9</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="21">
+        <v>3</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="26"/>
+      <c r="K25" s="27"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="20">
+        <v>10</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="21">
+        <v>3</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="26"/>
+      <c r="K26" s="27"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="10">
+        <v>11</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="11">
+        <v>2</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="27"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="23">
+        <v>12</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="24">
+        <v>4</v>
+      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="24"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="27"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="10">
+        <v>13</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="11">
+        <v>2</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="13">
+        <v>14</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="14">
+        <v>1</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="K30" s="29"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="13">
+        <v>15</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="14">
+        <v>1</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" s="14"/>
+      <c r="J31" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="29"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="20">
+        <v>16</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="21">
+        <v>3</v>
+      </c>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="21"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="27"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="13">
+        <v>17</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="14">
+        <v>1</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="14"/>
+      <c r="J33" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="29"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="20">
+        <v>18</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="21">
+        <v>3</v>
+      </c>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J34" s="26"/>
+      <c r="K34" s="27"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="20">
+        <v>19</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="21">
+        <v>3</v>
+      </c>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J35" s="26"/>
+      <c r="K35" s="27"/>
+    </row>
   </sheetData>
+  <sortState ref="A17:E35">
+    <sortCondition ref="A17"/>
+  </sortState>
+  <mergeCells count="21">
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -828,7 +1625,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -840,7 +1637,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>